<commit_message>
calories app complete for now
</commit_message>
<xml_diff>
--- a/datasets/calories_11042022.xlsx
+++ b/datasets/calories_11042022.xlsx
@@ -504,7 +504,9 @@
       <c r="G2" t="n">
         <v>35000</v>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -530,7 +532,9 @@
       <c r="G3" t="n">
         <v>34625</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -556,7 +560,9 @@
       <c r="G4" t="n">
         <v>34250</v>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -582,7 +588,9 @@
       <c r="G5" t="n">
         <v>33875</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -608,7 +616,9 @@
       <c r="G6" t="n">
         <v>33500</v>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -634,7 +644,9 @@
       <c r="G7" t="n">
         <v>33125</v>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -660,7 +672,9 @@
       <c r="G8" t="n">
         <v>32750</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -686,7 +700,9 @@
       <c r="G9" t="n">
         <v>32375</v>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -712,7 +728,9 @@
       <c r="G10" t="n">
         <v>32000</v>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -738,7 +756,9 @@
       <c r="G11" t="n">
         <v>31625</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -764,7 +784,9 @@
       <c r="G12" t="n">
         <v>31250</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -790,7 +812,9 @@
       <c r="G13" t="n">
         <v>30875</v>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -816,7 +840,9 @@
       <c r="G14" t="n">
         <v>30500</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -842,7 +868,9 @@
       <c r="G15" t="n">
         <v>30125</v>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -868,7 +896,9 @@
       <c r="G16" t="n">
         <v>29750</v>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -894,7 +924,9 @@
       <c r="G17" t="n">
         <v>29375</v>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -920,7 +952,9 @@
       <c r="G18" t="n">
         <v>29000</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -946,7 +980,9 @@
       <c r="G19" t="n">
         <v>28625</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -972,7 +1008,9 @@
       <c r="G20" t="n">
         <v>28250</v>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -998,7 +1036,9 @@
       <c r="G21" t="n">
         <v>27875</v>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1024,7 +1064,9 @@
       <c r="G22" t="n">
         <v>27500</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1050,7 +1092,9 @@
       <c r="G23" t="n">
         <v>27125</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1076,7 +1120,9 @@
       <c r="G24" t="n">
         <v>26750</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1102,7 +1148,9 @@
       <c r="G25" t="n">
         <v>26375</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1128,7 +1176,9 @@
       <c r="G26" t="n">
         <v>26000</v>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1154,7 +1204,9 @@
       <c r="G27" t="n">
         <v>25625</v>
       </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1180,7 +1232,9 @@
       <c r="G28" t="n">
         <v>25250</v>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1206,7 +1260,9 @@
       <c r="G29" t="n">
         <v>24875</v>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1232,7 +1288,9 @@
       <c r="G30" t="n">
         <v>24500</v>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1258,7 +1316,9 @@
       <c r="G31" t="n">
         <v>24125</v>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1284,7 +1344,9 @@
       <c r="G32" t="n">
         <v>23750</v>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1310,7 +1372,9 @@
       <c r="G33" t="n">
         <v>23375</v>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1336,7 +1400,9 @@
       <c r="G34" t="n">
         <v>23000</v>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1366,7 +1432,9 @@
       <c r="G35" t="n">
         <v>22625</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1428,7 +1496,9 @@
       <c r="G37" t="n">
         <v>21875</v>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1458,7 +1528,9 @@
       <c r="G38" t="n">
         <v>21500</v>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -1484,7 +1556,9 @@
       <c r="G39" t="n">
         <v>21125</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -1510,7 +1584,9 @@
       <c r="G40" t="n">
         <v>20750</v>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -1536,7 +1612,9 @@
       <c r="G41" t="n">
         <v>20375</v>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1562,7 +1640,9 @@
       <c r="G42" t="n">
         <v>20000</v>
       </c>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1583,10 +1663,8 @@
       <c r="D43" s="2" t="n">
         <v>44876</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>-500</t>
-        </is>
+      <c r="E43" t="n">
+        <v>-500</v>
       </c>
       <c r="F43" t="n">
         <v>24924</v>
@@ -1594,7 +1672,9 @@
       <c r="G43" t="n">
         <v>19625</v>
       </c>
-      <c r="H43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1620,7 +1700,9 @@
       <c r="G44" t="n">
         <v>19250</v>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1633,12 +1715,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D45" s="2" t="n">
         <v>44878</v>
       </c>
       <c r="E45" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>22224</v>
@@ -1646,7 +1732,9 @@
       <c r="G45" t="n">
         <v>18875</v>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -1672,7 +1760,9 @@
       <c r="G46" t="n">
         <v>18500</v>
       </c>
-      <c r="H46" t="inlineStr"/>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1698,7 +1788,9 @@
       <c r="G47" t="n">
         <v>18125</v>
       </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1724,7 +1816,9 @@
       <c r="G48" t="n">
         <v>17750</v>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1750,7 +1844,9 @@
       <c r="G49" t="n">
         <v>17375</v>
       </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1776,7 +1872,9 @@
       <c r="G50" t="n">
         <v>17000</v>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1802,7 +1900,9 @@
       <c r="G51" t="n">
         <v>16625</v>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1815,12 +1915,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D52" s="2" t="n">
         <v>44885</v>
       </c>
       <c r="E52" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
         <v>19524</v>
@@ -1828,7 +1932,9 @@
       <c r="G52" t="n">
         <v>16250</v>
       </c>
-      <c r="H52" t="inlineStr"/>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1854,7 +1960,9 @@
       <c r="G53" t="n">
         <v>15875</v>
       </c>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1880,7 +1988,9 @@
       <c r="G54" t="n">
         <v>15500</v>
       </c>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -1906,7 +2016,9 @@
       <c r="G55" t="n">
         <v>15125</v>
       </c>
-      <c r="H55" t="inlineStr"/>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -1919,7 +2031,11 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D56" s="2" t="n">
         <v>44889</v>
       </c>
@@ -1932,7 +2048,9 @@
       <c r="G56" t="n">
         <v>14750</v>
       </c>
-      <c r="H56" t="inlineStr"/>
+      <c r="H56" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -1958,7 +2076,9 @@
       <c r="G57" t="n">
         <v>14375</v>
       </c>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1984,7 +2104,9 @@
       <c r="G58" t="n">
         <v>14000</v>
       </c>
-      <c r="H58" t="inlineStr"/>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1997,12 +2119,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D59" s="2" t="n">
         <v>44892</v>
       </c>
       <c r="E59" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
         <v>18824</v>
@@ -2010,7 +2136,9 @@
       <c r="G59" t="n">
         <v>13625</v>
       </c>
-      <c r="H59" t="inlineStr"/>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -2036,7 +2164,9 @@
       <c r="G60" t="n">
         <v>13250</v>
       </c>
-      <c r="H60" t="inlineStr"/>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -2062,7 +2192,9 @@
       <c r="G61" t="n">
         <v>12875</v>
       </c>
-      <c r="H61" t="inlineStr"/>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -2088,7 +2220,9 @@
       <c r="G62" t="n">
         <v>12500</v>
       </c>
-      <c r="H62" t="inlineStr"/>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -2114,7 +2248,9 @@
       <c r="G63" t="n">
         <v>12125</v>
       </c>
-      <c r="H63" t="inlineStr"/>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -2140,7 +2276,9 @@
       <c r="G64" t="n">
         <v>11750</v>
       </c>
-      <c r="H64" t="inlineStr"/>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -2166,7 +2304,9 @@
       <c r="G65" t="n">
         <v>11375</v>
       </c>
-      <c r="H65" t="inlineStr"/>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -2179,12 +2319,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D66" s="2" t="n">
         <v>44899</v>
       </c>
       <c r="E66" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
         <v>16124</v>
@@ -2192,7 +2336,9 @@
       <c r="G66" t="n">
         <v>11000</v>
       </c>
-      <c r="H66" t="inlineStr"/>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -2218,7 +2364,9 @@
       <c r="G67" t="n">
         <v>10625</v>
       </c>
-      <c r="H67" t="inlineStr"/>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -2244,7 +2392,9 @@
       <c r="G68" t="n">
         <v>10250</v>
       </c>
-      <c r="H68" t="inlineStr"/>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -2270,7 +2420,9 @@
       <c r="G69" t="n">
         <v>9875</v>
       </c>
-      <c r="H69" t="inlineStr"/>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -2296,7 +2448,9 @@
       <c r="G70" t="n">
         <v>9500</v>
       </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -2322,7 +2476,9 @@
       <c r="G71" t="n">
         <v>9125</v>
       </c>
-      <c r="H71" t="inlineStr"/>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -2348,7 +2504,9 @@
       <c r="G72" t="n">
         <v>8750</v>
       </c>
-      <c r="H72" t="inlineStr"/>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -2361,12 +2519,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D73" s="2" t="n">
         <v>44906</v>
       </c>
       <c r="E73" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
         <v>13424</v>
@@ -2374,7 +2536,9 @@
       <c r="G73" t="n">
         <v>8375</v>
       </c>
-      <c r="H73" t="inlineStr"/>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -2400,7 +2564,9 @@
       <c r="G74" t="n">
         <v>8000</v>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -2426,7 +2592,9 @@
       <c r="G75" t="n">
         <v>7625</v>
       </c>
-      <c r="H75" t="inlineStr"/>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -2452,7 +2620,9 @@
       <c r="G76" t="n">
         <v>7250</v>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -2478,7 +2648,9 @@
       <c r="G77" t="n">
         <v>6875</v>
       </c>
-      <c r="H77" t="inlineStr"/>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -2504,7 +2676,9 @@
       <c r="G78" t="n">
         <v>6500</v>
       </c>
-      <c r="H78" t="inlineStr"/>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2530,7 +2704,9 @@
       <c r="G79" t="n">
         <v>6125</v>
       </c>
-      <c r="H79" t="inlineStr"/>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -2543,12 +2719,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D80" s="2" t="n">
         <v>44913</v>
       </c>
       <c r="E80" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
         <v>10724</v>
@@ -2556,7 +2736,9 @@
       <c r="G80" t="n">
         <v>5750</v>
       </c>
-      <c r="H80" t="inlineStr"/>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -2582,7 +2764,9 @@
       <c r="G81" t="n">
         <v>5375</v>
       </c>
-      <c r="H81" t="inlineStr"/>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -2608,7 +2792,9 @@
       <c r="G82" t="n">
         <v>5000</v>
       </c>
-      <c r="H82" t="inlineStr"/>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -2634,7 +2820,9 @@
       <c r="G83" t="n">
         <v>4625</v>
       </c>
-      <c r="H83" t="inlineStr"/>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -2660,7 +2848,9 @@
       <c r="G84" t="n">
         <v>4250</v>
       </c>
-      <c r="H84" t="inlineStr"/>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -2673,7 +2863,11 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D85" s="2" t="n">
         <v>44918</v>
       </c>
@@ -2686,7 +2880,9 @@
       <c r="G85" t="n">
         <v>3875</v>
       </c>
-      <c r="H85" t="inlineStr"/>
+      <c r="H85" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -2699,7 +2895,11 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D86" s="2" t="n">
         <v>44919</v>
       </c>
@@ -2712,7 +2912,11 @@
       <c r="G86" t="n">
         <v>3500</v>
       </c>
-      <c r="H86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -2725,12 +2929,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D87" s="2" t="n">
         <v>44920</v>
       </c>
       <c r="E87" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F87" t="n">
         <v>14024</v>
@@ -2738,7 +2946,9 @@
       <c r="G87" t="n">
         <v>3125</v>
       </c>
-      <c r="H87" t="inlineStr"/>
+      <c r="H87" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -2764,7 +2974,9 @@
       <c r="G88" t="n">
         <v>2750</v>
       </c>
-      <c r="H88" t="inlineStr"/>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -2790,7 +3002,9 @@
       <c r="G89" t="n">
         <v>2375</v>
       </c>
-      <c r="H89" t="inlineStr"/>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -2816,7 +3030,9 @@
       <c r="G90" t="n">
         <v>2000</v>
       </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -2842,7 +3058,9 @@
       <c r="G91" t="n">
         <v>1625</v>
       </c>
-      <c r="H91" t="inlineStr"/>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -2868,7 +3086,9 @@
       <c r="G92" t="n">
         <v>1250</v>
       </c>
-      <c r="H92" t="inlineStr"/>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -2894,7 +3114,9 @@
       <c r="G93" t="n">
         <v>875</v>
       </c>
-      <c r="H93" t="inlineStr"/>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
@@ -2907,12 +3129,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>11/13/2022</t>
+        </is>
+      </c>
       <c r="D94" s="2" t="n">
         <v>44927</v>
       </c>
       <c r="E94" t="n">
-        <v>-2700</v>
+        <v>0</v>
       </c>
       <c r="F94" t="n">
         <v>11324</v>
@@ -2920,7 +3146,9 @@
       <c r="G94" t="n">
         <v>500</v>
       </c>
-      <c r="H94" t="inlineStr"/>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Body fat day update
</commit_message>
<xml_diff>
--- a/datasets/calories_11042022.xlsx
+++ b/datasets/calories_11042022.xlsx
@@ -504,8 +504,10 @@
       <c r="G2" t="n">
         <v>35000</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -532,8 +534,10 @@
       <c r="G3" t="n">
         <v>34625</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -560,8 +564,10 @@
       <c r="G4" t="n">
         <v>34250</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -588,8 +594,10 @@
       <c r="G5" t="n">
         <v>33875</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -616,8 +624,10 @@
       <c r="G6" t="n">
         <v>33500</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -644,8 +654,10 @@
       <c r="G7" t="n">
         <v>33125</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -672,8 +684,10 @@
       <c r="G8" t="n">
         <v>32750</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -700,8 +714,10 @@
       <c r="G9" t="n">
         <v>32375</v>
       </c>
-      <c r="H9" t="n">
-        <v>0</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -728,8 +744,10 @@
       <c r="G10" t="n">
         <v>32000</v>
       </c>
-      <c r="H10" t="n">
-        <v>0</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -756,8 +774,10 @@
       <c r="G11" t="n">
         <v>31625</v>
       </c>
-      <c r="H11" t="n">
-        <v>0</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -784,8 +804,10 @@
       <c r="G12" t="n">
         <v>31250</v>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -812,8 +834,10 @@
       <c r="G13" t="n">
         <v>30875</v>
       </c>
-      <c r="H13" t="n">
-        <v>0</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -840,8 +864,10 @@
       <c r="G14" t="n">
         <v>30500</v>
       </c>
-      <c r="H14" t="n">
-        <v>0</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -868,8 +894,10 @@
       <c r="G15" t="n">
         <v>30125</v>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -896,8 +924,10 @@
       <c r="G16" t="n">
         <v>29750</v>
       </c>
-      <c r="H16" t="n">
-        <v>0</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -924,8 +954,10 @@
       <c r="G17" t="n">
         <v>29375</v>
       </c>
-      <c r="H17" t="n">
-        <v>0</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -952,8 +984,10 @@
       <c r="G18" t="n">
         <v>29000</v>
       </c>
-      <c r="H18" t="n">
-        <v>0</v>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -980,8 +1014,10 @@
       <c r="G19" t="n">
         <v>28625</v>
       </c>
-      <c r="H19" t="n">
-        <v>0</v>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1008,8 +1044,10 @@
       <c r="G20" t="n">
         <v>28250</v>
       </c>
-      <c r="H20" t="n">
-        <v>0</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1036,8 +1074,10 @@
       <c r="G21" t="n">
         <v>27875</v>
       </c>
-      <c r="H21" t="n">
-        <v>0</v>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1064,8 +1104,10 @@
       <c r="G22" t="n">
         <v>27500</v>
       </c>
-      <c r="H22" t="n">
-        <v>0</v>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1092,8 +1134,10 @@
       <c r="G23" t="n">
         <v>27125</v>
       </c>
-      <c r="H23" t="n">
-        <v>0</v>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1120,8 +1164,10 @@
       <c r="G24" t="n">
         <v>26750</v>
       </c>
-      <c r="H24" t="n">
-        <v>0</v>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1148,8 +1194,10 @@
       <c r="G25" t="n">
         <v>26375</v>
       </c>
-      <c r="H25" t="n">
-        <v>0</v>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1176,8 +1224,10 @@
       <c r="G26" t="n">
         <v>26000</v>
       </c>
-      <c r="H26" t="n">
-        <v>0</v>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1204,8 +1254,10 @@
       <c r="G27" t="n">
         <v>25625</v>
       </c>
-      <c r="H27" t="n">
-        <v>0</v>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1232,8 +1284,10 @@
       <c r="G28" t="n">
         <v>25250</v>
       </c>
-      <c r="H28" t="n">
-        <v>0</v>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1260,8 +1314,10 @@
       <c r="G29" t="n">
         <v>24875</v>
       </c>
-      <c r="H29" t="n">
-        <v>0</v>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1288,8 +1344,10 @@
       <c r="G30" t="n">
         <v>24500</v>
       </c>
-      <c r="H30" t="n">
-        <v>0</v>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1316,8 +1374,10 @@
       <c r="G31" t="n">
         <v>24125</v>
       </c>
-      <c r="H31" t="n">
-        <v>0</v>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1344,8 +1404,10 @@
       <c r="G32" t="n">
         <v>23750</v>
       </c>
-      <c r="H32" t="n">
-        <v>0</v>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1372,8 +1434,10 @@
       <c r="G33" t="n">
         <v>23375</v>
       </c>
-      <c r="H33" t="n">
-        <v>0</v>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1400,8 +1464,10 @@
       <c r="G34" t="n">
         <v>23000</v>
       </c>
-      <c r="H34" t="n">
-        <v>0</v>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -1432,8 +1498,10 @@
       <c r="G35" t="n">
         <v>22625</v>
       </c>
-      <c r="H35" t="n">
-        <v>0</v>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1464,8 +1532,10 @@
       <c r="G36" t="n">
         <v>22250</v>
       </c>
-      <c r="H36" t="n">
-        <v>500</v>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1496,8 +1566,10 @@
       <c r="G37" t="n">
         <v>21875</v>
       </c>
-      <c r="H37" t="n">
-        <v>0</v>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1528,8 +1600,10 @@
       <c r="G38" t="n">
         <v>21500</v>
       </c>
-      <c r="H38" t="n">
-        <v>0</v>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1556,8 +1630,10 @@
       <c r="G39" t="n">
         <v>21125</v>
       </c>
-      <c r="H39" t="n">
-        <v>0</v>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1584,8 +1660,10 @@
       <c r="G40" t="n">
         <v>20750</v>
       </c>
-      <c r="H40" t="n">
-        <v>0</v>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1612,8 +1690,10 @@
       <c r="G41" t="n">
         <v>20375</v>
       </c>
-      <c r="H41" t="n">
-        <v>0</v>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1640,8 +1720,10 @@
       <c r="G42" t="n">
         <v>20000</v>
       </c>
-      <c r="H42" t="n">
-        <v>0</v>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1672,8 +1754,10 @@
       <c r="G43" t="n">
         <v>19625</v>
       </c>
-      <c r="H43" t="n">
-        <v>0</v>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1700,8 +1784,10 @@
       <c r="G44" t="n">
         <v>19250</v>
       </c>
-      <c r="H44" t="n">
-        <v>0</v>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1717,14 +1803,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11/13/2022</t>
+          <t>11/14/2022</t>
         </is>
       </c>
       <c r="D45" s="2" t="n">
         <v>44878</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>-1100</v>
       </c>
       <c r="F45" t="n">
         <v>22224</v>
@@ -1732,8 +1818,10 @@
       <c r="G45" t="n">
         <v>18875</v>
       </c>
-      <c r="H45" t="n">
-        <v>0</v>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1760,8 +1848,10 @@
       <c r="G46" t="n">
         <v>18500</v>
       </c>
-      <c r="H46" t="n">
-        <v>0</v>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1788,8 +1878,10 @@
       <c r="G47" t="n">
         <v>18125</v>
       </c>
-      <c r="H47" t="n">
-        <v>0</v>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1816,8 +1908,10 @@
       <c r="G48" t="n">
         <v>17750</v>
       </c>
-      <c r="H48" t="n">
-        <v>0</v>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1844,8 +1938,10 @@
       <c r="G49" t="n">
         <v>17375</v>
       </c>
-      <c r="H49" t="n">
-        <v>0</v>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1872,8 +1968,10 @@
       <c r="G50" t="n">
         <v>17000</v>
       </c>
-      <c r="H50" t="n">
-        <v>0</v>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1900,8 +1998,10 @@
       <c r="G51" t="n">
         <v>16625</v>
       </c>
-      <c r="H51" t="n">
-        <v>0</v>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1932,8 +2032,10 @@
       <c r="G52" t="n">
         <v>16250</v>
       </c>
-      <c r="H52" t="n">
-        <v>0</v>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1960,8 +2062,10 @@
       <c r="G53" t="n">
         <v>15875</v>
       </c>
-      <c r="H53" t="n">
-        <v>0</v>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1988,8 +2092,10 @@
       <c r="G54" t="n">
         <v>15500</v>
       </c>
-      <c r="H54" t="n">
-        <v>0</v>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -2016,8 +2122,10 @@
       <c r="G55" t="n">
         <v>15125</v>
       </c>
-      <c r="H55" t="n">
-        <v>0</v>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -2048,8 +2156,10 @@
       <c r="G56" t="n">
         <v>14750</v>
       </c>
-      <c r="H56" t="n">
-        <v>1000</v>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -2076,8 +2186,10 @@
       <c r="G57" t="n">
         <v>14375</v>
       </c>
-      <c r="H57" t="n">
-        <v>0</v>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -2104,8 +2216,10 @@
       <c r="G58" t="n">
         <v>14000</v>
       </c>
-      <c r="H58" t="n">
-        <v>0</v>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -2136,8 +2250,10 @@
       <c r="G59" t="n">
         <v>13625</v>
       </c>
-      <c r="H59" t="n">
-        <v>0</v>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -2164,8 +2280,10 @@
       <c r="G60" t="n">
         <v>13250</v>
       </c>
-      <c r="H60" t="n">
-        <v>0</v>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -2192,8 +2310,10 @@
       <c r="G61" t="n">
         <v>12875</v>
       </c>
-      <c r="H61" t="n">
-        <v>0</v>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -2220,8 +2340,10 @@
       <c r="G62" t="n">
         <v>12500</v>
       </c>
-      <c r="H62" t="n">
-        <v>0</v>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -2248,8 +2370,10 @@
       <c r="G63" t="n">
         <v>12125</v>
       </c>
-      <c r="H63" t="n">
-        <v>0</v>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -2276,8 +2400,10 @@
       <c r="G64" t="n">
         <v>11750</v>
       </c>
-      <c r="H64" t="n">
-        <v>0</v>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -2304,8 +2430,10 @@
       <c r="G65" t="n">
         <v>11375</v>
       </c>
-      <c r="H65" t="n">
-        <v>0</v>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -2336,8 +2464,10 @@
       <c r="G66" t="n">
         <v>11000</v>
       </c>
-      <c r="H66" t="n">
-        <v>0</v>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -2364,8 +2494,10 @@
       <c r="G67" t="n">
         <v>10625</v>
       </c>
-      <c r="H67" t="n">
-        <v>0</v>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -2392,8 +2524,10 @@
       <c r="G68" t="n">
         <v>10250</v>
       </c>
-      <c r="H68" t="n">
-        <v>0</v>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -2420,8 +2554,10 @@
       <c r="G69" t="n">
         <v>9875</v>
       </c>
-      <c r="H69" t="n">
-        <v>0</v>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -2448,8 +2584,10 @@
       <c r="G70" t="n">
         <v>9500</v>
       </c>
-      <c r="H70" t="n">
-        <v>0</v>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -2476,8 +2614,10 @@
       <c r="G71" t="n">
         <v>9125</v>
       </c>
-      <c r="H71" t="n">
-        <v>0</v>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -2504,8 +2644,10 @@
       <c r="G72" t="n">
         <v>8750</v>
       </c>
-      <c r="H72" t="n">
-        <v>0</v>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -2536,8 +2678,10 @@
       <c r="G73" t="n">
         <v>8375</v>
       </c>
-      <c r="H73" t="n">
-        <v>0</v>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -2564,8 +2708,10 @@
       <c r="G74" t="n">
         <v>8000</v>
       </c>
-      <c r="H74" t="n">
-        <v>0</v>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -2592,8 +2738,10 @@
       <c r="G75" t="n">
         <v>7625</v>
       </c>
-      <c r="H75" t="n">
-        <v>0</v>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -2620,8 +2768,10 @@
       <c r="G76" t="n">
         <v>7250</v>
       </c>
-      <c r="H76" t="n">
-        <v>0</v>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -2648,8 +2798,10 @@
       <c r="G77" t="n">
         <v>6875</v>
       </c>
-      <c r="H77" t="n">
-        <v>0</v>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -2676,8 +2828,10 @@
       <c r="G78" t="n">
         <v>6500</v>
       </c>
-      <c r="H78" t="n">
-        <v>0</v>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -2704,8 +2858,10 @@
       <c r="G79" t="n">
         <v>6125</v>
       </c>
-      <c r="H79" t="n">
-        <v>0</v>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -2736,8 +2892,10 @@
       <c r="G80" t="n">
         <v>5750</v>
       </c>
-      <c r="H80" t="n">
-        <v>0</v>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="81">
@@ -2764,8 +2922,10 @@
       <c r="G81" t="n">
         <v>5375</v>
       </c>
-      <c r="H81" t="n">
-        <v>0</v>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="82">
@@ -2792,8 +2952,10 @@
       <c r="G82" t="n">
         <v>5000</v>
       </c>
-      <c r="H82" t="n">
-        <v>0</v>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -2820,8 +2982,10 @@
       <c r="G83" t="n">
         <v>4625</v>
       </c>
-      <c r="H83" t="n">
-        <v>0</v>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -2848,8 +3012,10 @@
       <c r="G84" t="n">
         <v>4250</v>
       </c>
-      <c r="H84" t="n">
-        <v>0</v>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -2880,8 +3046,10 @@
       <c r="G85" t="n">
         <v>3875</v>
       </c>
-      <c r="H85" t="n">
-        <v>1000</v>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -2946,8 +3114,10 @@
       <c r="G87" t="n">
         <v>3125</v>
       </c>
-      <c r="H87" t="n">
-        <v>1000</v>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -2974,8 +3144,10 @@
       <c r="G88" t="n">
         <v>2750</v>
       </c>
-      <c r="H88" t="n">
-        <v>0</v>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -3002,8 +3174,10 @@
       <c r="G89" t="n">
         <v>2375</v>
       </c>
-      <c r="H89" t="n">
-        <v>0</v>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="90">
@@ -3030,8 +3204,10 @@
       <c r="G90" t="n">
         <v>2000</v>
       </c>
-      <c r="H90" t="n">
-        <v>0</v>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="91">
@@ -3058,8 +3234,10 @@
       <c r="G91" t="n">
         <v>1625</v>
       </c>
-      <c r="H91" t="n">
-        <v>0</v>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -3086,8 +3264,10 @@
       <c r="G92" t="n">
         <v>1250</v>
       </c>
-      <c r="H92" t="n">
-        <v>0</v>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -3114,8 +3294,10 @@
       <c r="G93" t="n">
         <v>875</v>
       </c>
-      <c r="H93" t="n">
-        <v>0</v>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="94">
@@ -3146,8 +3328,10 @@
       <c r="G94" t="n">
         <v>500</v>
       </c>
-      <c r="H94" t="n">
-        <v>0</v>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apply() and exec() test
</commit_message>
<xml_diff>
--- a/datasets/calories_11042022.xlsx
+++ b/datasets/calories_11042022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="headers" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="headers" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -504,10 +504,8 @@
       <c r="G2" t="n">
         <v>35000</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -534,10 +532,8 @@
       <c r="G3" t="n">
         <v>34625</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -564,10 +560,8 @@
       <c r="G4" t="n">
         <v>34250</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -594,10 +588,8 @@
       <c r="G5" t="n">
         <v>33875</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -624,10 +616,8 @@
       <c r="G6" t="n">
         <v>33500</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -654,10 +644,8 @@
       <c r="G7" t="n">
         <v>33125</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -684,10 +672,8 @@
       <c r="G8" t="n">
         <v>32750</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -714,10 +700,8 @@
       <c r="G9" t="n">
         <v>32375</v>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -744,10 +728,8 @@
       <c r="G10" t="n">
         <v>32000</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -774,10 +756,8 @@
       <c r="G11" t="n">
         <v>31625</v>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -804,10 +784,8 @@
       <c r="G12" t="n">
         <v>31250</v>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -834,10 +812,8 @@
       <c r="G13" t="n">
         <v>30875</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -864,10 +840,8 @@
       <c r="G14" t="n">
         <v>30500</v>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -894,10 +868,8 @@
       <c r="G15" t="n">
         <v>30125</v>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -924,10 +896,8 @@
       <c r="G16" t="n">
         <v>29750</v>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -954,10 +924,8 @@
       <c r="G17" t="n">
         <v>29375</v>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -984,10 +952,8 @@
       <c r="G18" t="n">
         <v>29000</v>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1014,10 +980,8 @@
       <c r="G19" t="n">
         <v>28625</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1044,10 +1008,8 @@
       <c r="G20" t="n">
         <v>28250</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1074,10 +1036,8 @@
       <c r="G21" t="n">
         <v>27875</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1104,10 +1064,8 @@
       <c r="G22" t="n">
         <v>27500</v>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1134,10 +1092,8 @@
       <c r="G23" t="n">
         <v>27125</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1164,10 +1120,8 @@
       <c r="G24" t="n">
         <v>26750</v>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1194,10 +1148,8 @@
       <c r="G25" t="n">
         <v>26375</v>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1224,10 +1176,8 @@
       <c r="G26" t="n">
         <v>26000</v>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1254,10 +1204,8 @@
       <c r="G27" t="n">
         <v>25625</v>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1284,10 +1232,8 @@
       <c r="G28" t="n">
         <v>25250</v>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1314,10 +1260,8 @@
       <c r="G29" t="n">
         <v>24875</v>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1344,10 +1288,8 @@
       <c r="G30" t="n">
         <v>24500</v>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1374,10 +1316,8 @@
       <c r="G31" t="n">
         <v>24125</v>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1404,10 +1344,8 @@
       <c r="G32" t="n">
         <v>23750</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1434,10 +1372,8 @@
       <c r="G33" t="n">
         <v>23375</v>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1464,10 +1400,8 @@
       <c r="G34" t="n">
         <v>23000</v>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1498,10 +1432,8 @@
       <c r="G35" t="n">
         <v>22625</v>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1532,10 +1464,8 @@
       <c r="G36" t="n">
         <v>22250</v>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="H36" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="37">
@@ -1566,10 +1496,8 @@
       <c r="G37" t="n">
         <v>21875</v>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1600,10 +1528,8 @@
       <c r="G38" t="n">
         <v>21500</v>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1630,10 +1556,8 @@
       <c r="G39" t="n">
         <v>21125</v>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1660,10 +1584,8 @@
       <c r="G40" t="n">
         <v>20750</v>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1690,10 +1612,8 @@
       <c r="G41" t="n">
         <v>20375</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1720,10 +1640,8 @@
       <c r="G42" t="n">
         <v>20000</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1754,10 +1672,8 @@
       <c r="G43" t="n">
         <v>19625</v>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1784,10 +1700,8 @@
       <c r="G44" t="n">
         <v>19250</v>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1818,10 +1732,8 @@
       <c r="G45" t="n">
         <v>18875</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1848,10 +1760,8 @@
       <c r="G46" t="n">
         <v>18500</v>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1878,10 +1788,8 @@
       <c r="G47" t="n">
         <v>18125</v>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1908,10 +1816,8 @@
       <c r="G48" t="n">
         <v>17750</v>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1938,10 +1844,8 @@
       <c r="G49" t="n">
         <v>17375</v>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1968,10 +1872,8 @@
       <c r="G50" t="n">
         <v>17000</v>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1985,12 +1887,18 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>11/26/2022</t>
+        </is>
+      </c>
       <c r="D51" s="2" t="n">
         <v>44884</v>
       </c>
-      <c r="E51" t="n">
-        <v>0</v>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>-1000</t>
+        </is>
       </c>
       <c r="F51" t="n">
         <v>22224</v>
@@ -1998,10 +1906,8 @@
       <c r="G51" t="n">
         <v>16625</v>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2032,10 +1938,8 @@
       <c r="G52" t="n">
         <v>16250</v>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2062,10 +1966,8 @@
       <c r="G53" t="n">
         <v>15875</v>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2092,10 +1994,8 @@
       <c r="G54" t="n">
         <v>15500</v>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2109,12 +2009,16 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>11/26/2022</t>
+        </is>
+      </c>
       <c r="D55" s="2" t="n">
         <v>44888</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="F55" t="n">
         <v>19524</v>
@@ -2122,10 +2026,8 @@
       <c r="G55" t="n">
         <v>15125</v>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2156,10 +2058,8 @@
       <c r="G56" t="n">
         <v>14750</v>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="H56" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="57">
@@ -2186,10 +2086,8 @@
       <c r="G57" t="n">
         <v>14375</v>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2216,10 +2114,8 @@
       <c r="G58" t="n">
         <v>14000</v>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2250,10 +2146,8 @@
       <c r="G59" t="n">
         <v>13625</v>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2280,10 +2174,8 @@
       <c r="G60" t="n">
         <v>13250</v>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2310,10 +2202,8 @@
       <c r="G61" t="n">
         <v>12875</v>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2340,10 +2230,8 @@
       <c r="G62" t="n">
         <v>12500</v>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2370,10 +2258,8 @@
       <c r="G63" t="n">
         <v>12125</v>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2400,10 +2286,8 @@
       <c r="G64" t="n">
         <v>11750</v>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2430,10 +2314,8 @@
       <c r="G65" t="n">
         <v>11375</v>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2464,10 +2346,8 @@
       <c r="G66" t="n">
         <v>11000</v>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2494,10 +2374,8 @@
       <c r="G67" t="n">
         <v>10625</v>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2524,10 +2402,8 @@
       <c r="G68" t="n">
         <v>10250</v>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2554,10 +2430,8 @@
       <c r="G69" t="n">
         <v>9875</v>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2584,10 +2458,8 @@
       <c r="G70" t="n">
         <v>9500</v>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2614,10 +2486,8 @@
       <c r="G71" t="n">
         <v>9125</v>
       </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2644,10 +2514,8 @@
       <c r="G72" t="n">
         <v>8750</v>
       </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2678,10 +2546,8 @@
       <c r="G73" t="n">
         <v>8375</v>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2708,10 +2574,8 @@
       <c r="G74" t="n">
         <v>8000</v>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2738,10 +2602,8 @@
       <c r="G75" t="n">
         <v>7625</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2768,10 +2630,8 @@
       <c r="G76" t="n">
         <v>7250</v>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2798,10 +2658,8 @@
       <c r="G77" t="n">
         <v>6875</v>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2828,10 +2686,8 @@
       <c r="G78" t="n">
         <v>6500</v>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2858,10 +2714,8 @@
       <c r="G79" t="n">
         <v>6125</v>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2892,10 +2746,8 @@
       <c r="G80" t="n">
         <v>5750</v>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2922,10 +2774,8 @@
       <c r="G81" t="n">
         <v>5375</v>
       </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2952,10 +2802,8 @@
       <c r="G82" t="n">
         <v>5000</v>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2982,10 +2830,8 @@
       <c r="G83" t="n">
         <v>4625</v>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3012,10 +2858,8 @@
       <c r="G84" t="n">
         <v>4250</v>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3046,10 +2890,8 @@
       <c r="G85" t="n">
         <v>3875</v>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="H85" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="86">
@@ -3080,10 +2922,8 @@
       <c r="G86" t="n">
         <v>3500</v>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="H86" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="87">
@@ -3114,10 +2954,8 @@
       <c r="G87" t="n">
         <v>3125</v>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="H87" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="88">
@@ -3144,10 +2982,8 @@
       <c r="G88" t="n">
         <v>2750</v>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -3174,10 +3010,8 @@
       <c r="G89" t="n">
         <v>2375</v>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3204,10 +3038,8 @@
       <c r="G90" t="n">
         <v>2000</v>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3234,10 +3066,8 @@
       <c r="G91" t="n">
         <v>1625</v>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3264,10 +3094,8 @@
       <c r="G92" t="n">
         <v>1250</v>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3294,10 +3122,8 @@
       <c r="G93" t="n">
         <v>875</v>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3328,10 +3154,8 @@
       <c r="G94" t="n">
         <v>500</v>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="H94" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
object support: create, delete, select
</commit_message>
<xml_diff>
--- a/datasets/calories_11042022.xlsx
+++ b/datasets/calories_11042022.xlsx
@@ -2107,10 +2107,8 @@
       <c r="D58" s="2" t="n">
         <v>44891</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>-300</t>
-        </is>
+      <c r="E58" t="n">
+        <v>-300</v>
       </c>
       <c r="F58" t="n">
         <v>21524</v>
@@ -2277,12 +2275,18 @@
           <t>11/04/2022</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>12/03/2022</t>
+        </is>
+      </c>
       <c r="D64" s="2" t="n">
         <v>44897</v>
       </c>
-      <c r="E64" t="n">
-        <v>0</v>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>-500</t>
+        </is>
       </c>
       <c r="F64" t="n">
         <v>18824</v>

</xml_diff>

<commit_message>
loading and setting columns by type
</commit_message>
<xml_diff>
--- a/datasets/calories_11042022.xlsx
+++ b/datasets/calories_11042022.xlsx
@@ -2283,10 +2283,8 @@
       <c r="D64" s="2" t="n">
         <v>44897</v>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>-500</t>
-        </is>
+      <c r="E64" t="n">
+        <v>-500</v>
       </c>
       <c r="F64" t="n">
         <v>18824</v>
@@ -2339,14 +2337,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11/13/2022</t>
+          <t>12/05/2022</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
         <v>44899</v>
       </c>
-      <c r="E66" t="n">
-        <v>0</v>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>-900</t>
+        </is>
       </c>
       <c r="F66" t="n">
         <v>16124</v>

</xml_diff>